<commit_message>
Minor issue parse int fixed & Front in folders
</commit_message>
<xml_diff>
--- a/back/data/joueurs.xlsx
+++ b/back/data/joueurs.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="10" count="10">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="8" count="8">
   <x:si>
     <x:t>Nom</x:t>
   </x:si>
@@ -35,9 +35,6 @@
   </x:si>
   <x:si>
     <x:t>ben</x:t>
-  </x:si>
-  <x:si>
-    <x:t>11</x:t>
   </x:si>
   <x:si>
     <x:t>0</x:t>
@@ -449,14 +446,14 @@
       <x:c r="A4" s="0" t="s">
         <x:v>6</x:v>
       </x:c>
-      <x:c r="B4" s="0" t="s">
+      <x:c r="B4" s="0" t="n">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="C4" s="0" t="n">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="D4" s="0" t="s">
         <x:v>7</x:v>
-      </x:c>
-      <x:c r="C4" s="0" t="s">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="D4" s="0" t="s">
-        <x:v>8</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>